<commit_message>
update opt1 graphs and report
</commit_message>
<xml_diff>
--- a/misc/opt1.xlsx
+++ b/misc/opt1.xlsx
@@ -8,27 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanshtarev/Documents/Work/repos/rubik_solver/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C99EA7-AF9B-424A-85EF-8BCC9D2F553D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62694EAA-F212-EE45-8469-8C141DAC4A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1040" windowWidth="40800" windowHeight="24140" xr2:uid="{EAAB80E9-7C5A-234D-BF3F-DF62DD458500}"/>
+    <workbookView xWindow="38540" yWindow="-240" windowWidth="40800" windowHeight="25380" xr2:uid="{EAAB80E9-7C5A-234D-BF3F-DF62DD458500}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$4:$B$103</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$G$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$G$4:$G$103</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$4:$C$103</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$F$4:$F$103</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$G$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$G$4:$G$103</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$4:$B$103</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$4:$C$103</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$F$4:$F$103</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -138,9 +124,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1607,6 +1592,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1621,6 +1661,7 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:tailEnd type="triangle"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1670,6 +1711,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Render</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t> Time, ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1684,6 +1785,7 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:tailEnd type="triangle"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3233,6 +3335,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3247,6 +3404,7 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:tailEnd type="triangle"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3297,6 +3455,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000"/>
+                  <a:t>Render</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                  <a:t> Time, ms</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="2000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3311,6 +3529,7 @@
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
+            <a:tailEnd type="triangle"/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3337,6 +3556,7 @@
         <c:crossAx val="557635791"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4909,10 +5129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D7FD23-B911-0D40-9577-06D9A79B11E5}">
-  <dimension ref="B2:I103"/>
+  <dimension ref="B2:H103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="AH35" sqref="AH35"/>
+    <sheetView tabSelected="1" topLeftCell="I27" zoomScale="125" workbookViewId="0">
+      <selection activeCell="P71" sqref="P71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4926,2032 +5146,2031 @@
     <col min="9" max="9" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3" t="s">
+      <c r="D2" s="4"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>22</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>13</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>14</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>23</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>13</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>14</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>22</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>14</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>22</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>10</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>14</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>21</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>13</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>5</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>13</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>23</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>12</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>6</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>14</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>22</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>13</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>7</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>14</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>22</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>14</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>8</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>15</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>23</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>12</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>9</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>14</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>21</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>13</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>10</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>15</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
         <v>11</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>24</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>13</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>11</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>14</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="2">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>23</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>12</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>12</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>15</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="2">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>23</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>14</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>13</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>13</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>21</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>11</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>14</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>15</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>15</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>22</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>10</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>15</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>13</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>21</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>11</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>16</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>14</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>22</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>12</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>17</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>15</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>22</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>14</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>18</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>14</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>21</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>10</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>19</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>13</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>21</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>14</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>20</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>14</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>22</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>12</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>21</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>13</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>21</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>12</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>22</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>15</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>22</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>14</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>23</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>13</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>23</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>11</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>24</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>15</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>22</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>12</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>25</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>13</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>21</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>10</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>26</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>14</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>27</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>22</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>11</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>27</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>15</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>28</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>21</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>11</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>28</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>14</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>29</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>23</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>14</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>29</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>15</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>30</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>23</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>13</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>30</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
         <v>15</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>31</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>21</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>10</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>31</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>15</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>32</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>21</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>13</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>32</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="1">
         <v>13</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>33</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>21</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>11</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="1">
         <v>33</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="1">
         <v>15</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>34</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="1">
         <v>21</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="1">
         <v>12</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
         <v>34</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="1">
         <v>16</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>35</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>22</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>10</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>35</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
         <v>15</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>36</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>23</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <v>13</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>36</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>15</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>37</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>23</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>11</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>37</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
         <v>15</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>38</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>20</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>11</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>38</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>14</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>39</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>22</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>10</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>39</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>14</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>40</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>22</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>12</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <v>40</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>14</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>41</v>
       </c>
-      <c r="C44" s="2">
+      <c r="C44" s="1">
         <v>22</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="1">
         <v>13</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>41</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
         <v>15</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>42</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="1">
         <v>21</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45" s="1">
         <v>13</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>42</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>14</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>43</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="1">
         <v>19</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46" s="1">
         <v>12</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="1">
         <v>43</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
         <v>15</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>44</v>
       </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1">
         <v>21</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47" s="1">
         <v>13</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="1">
         <v>44</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
         <v>14</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>45</v>
       </c>
-      <c r="C48" s="2">
+      <c r="C48" s="1">
         <v>21</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48" s="1">
         <v>12</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="1">
         <v>45</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
         <v>14</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>46</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="1">
         <v>23</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49" s="1">
         <v>10</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="1">
         <v>46</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="1">
         <v>14</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>47</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="1">
         <v>22</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="1">
         <v>12</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="1">
         <v>47</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="1">
         <v>13</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>48</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="1">
         <v>21</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51" s="1">
         <v>10</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="1">
         <v>48</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="1">
         <v>14</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>49</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="1">
         <v>21</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="1">
         <v>11</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="1">
         <v>49</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="1">
         <v>14</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>50</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="1">
         <v>21</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53" s="1">
         <v>10</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="1">
         <v>50</v>
       </c>
-      <c r="G53" s="2">
+      <c r="G53" s="1">
         <v>13</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>51</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="1">
         <v>22</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54" s="1">
         <v>12</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="1">
         <v>51</v>
       </c>
-      <c r="G54" s="2">
+      <c r="G54" s="1">
         <v>14</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>52</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="1">
         <v>23</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <v>14</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="1">
         <v>52</v>
       </c>
-      <c r="G55" s="2">
+      <c r="G55" s="1">
         <v>13</v>
       </c>
-      <c r="H55" s="2">
+      <c r="H55" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>53</v>
       </c>
-      <c r="C56" s="2">
+      <c r="C56" s="1">
         <v>22</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56" s="1">
         <v>13</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="1">
         <v>53</v>
       </c>
-      <c r="G56" s="2">
+      <c r="G56" s="1">
         <v>15</v>
       </c>
-      <c r="H56" s="2">
+      <c r="H56" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>54</v>
       </c>
-      <c r="C57" s="2">
+      <c r="C57" s="1">
         <v>21</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57" s="1">
         <v>13</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="1">
         <v>54</v>
       </c>
-      <c r="G57" s="2">
+      <c r="G57" s="1">
         <v>13</v>
       </c>
-      <c r="H57" s="2">
+      <c r="H57" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>55</v>
       </c>
-      <c r="C58" s="2">
+      <c r="C58" s="1">
         <v>23</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="1">
         <v>13</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="1">
         <v>55</v>
       </c>
-      <c r="G58" s="2">
+      <c r="G58" s="1">
         <v>14</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>56</v>
       </c>
-      <c r="C59" s="2">
+      <c r="C59" s="1">
         <v>22</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="1">
         <v>13</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59" s="1">
         <v>56</v>
       </c>
-      <c r="G59" s="2">
+      <c r="G59" s="1">
         <v>14</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>57</v>
       </c>
-      <c r="C60" s="2">
+      <c r="C60" s="1">
         <v>22</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60" s="1">
         <v>13</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="1">
         <v>57</v>
       </c>
-      <c r="G60" s="2">
+      <c r="G60" s="1">
         <v>15</v>
       </c>
-      <c r="H60" s="2">
+      <c r="H60" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>58</v>
       </c>
-      <c r="C61" s="2">
+      <c r="C61" s="1">
         <v>22</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="1">
         <v>10</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61" s="1">
         <v>58</v>
       </c>
-      <c r="G61" s="2">
+      <c r="G61" s="1">
         <v>15</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>59</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="1">
         <v>21</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="1">
         <v>10</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="1">
         <v>59</v>
       </c>
-      <c r="G62" s="2">
+      <c r="G62" s="1">
         <v>13</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>60</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="1">
         <v>23</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63" s="1">
         <v>13</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="1">
         <v>60</v>
       </c>
-      <c r="G63" s="2">
+      <c r="G63" s="1">
         <v>13</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>61</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="1">
         <v>22</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="1">
         <v>11</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <v>61</v>
       </c>
-      <c r="G64" s="2">
+      <c r="G64" s="1">
         <v>13</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>62</v>
       </c>
-      <c r="C65" s="2">
+      <c r="C65" s="1">
         <v>23</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="1">
         <v>10</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="1">
         <v>62</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G65" s="1">
         <v>14</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>63</v>
       </c>
-      <c r="C66" s="2">
+      <c r="C66" s="1">
         <v>23</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="1">
         <v>11</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="1">
         <v>63</v>
       </c>
-      <c r="G66" s="2">
+      <c r="G66" s="1">
         <v>14</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>64</v>
       </c>
-      <c r="C67" s="2">
+      <c r="C67" s="1">
         <v>23</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="1">
         <v>10</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="1">
         <v>64</v>
       </c>
-      <c r="G67" s="2">
+      <c r="G67" s="1">
         <v>13</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>65</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="1">
         <v>21</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="1">
         <v>10</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="1">
         <v>65</v>
       </c>
-      <c r="G68" s="2">
+      <c r="G68" s="1">
         <v>14</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>66</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="1">
         <v>23</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="1">
         <v>12</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="1">
         <v>66</v>
       </c>
-      <c r="G69" s="2">
+      <c r="G69" s="1">
         <v>13</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>67</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="1">
         <v>22</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70" s="1">
         <v>13</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70" s="1">
         <v>67</v>
       </c>
-      <c r="G70" s="2">
+      <c r="G70" s="1">
         <v>15</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>68</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="1">
         <v>21</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="1">
         <v>14</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="1">
         <v>68</v>
       </c>
-      <c r="G71" s="2">
+      <c r="G71" s="1">
         <v>13</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>69</v>
       </c>
-      <c r="C72" s="2">
+      <c r="C72" s="1">
         <v>23</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72" s="1">
         <v>12</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="1">
         <v>69</v>
       </c>
-      <c r="G72" s="2">
+      <c r="G72" s="1">
         <v>14</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>70</v>
       </c>
-      <c r="C73" s="2">
+      <c r="C73" s="1">
         <v>22</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="1">
         <v>14</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="1">
         <v>70</v>
       </c>
-      <c r="G73" s="2">
+      <c r="G73" s="1">
         <v>13</v>
       </c>
-      <c r="H73" s="2">
+      <c r="H73" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>71</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="1">
         <v>21</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74" s="1">
         <v>13</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74" s="1">
         <v>71</v>
       </c>
-      <c r="G74" s="2">
+      <c r="G74" s="1">
         <v>15</v>
       </c>
-      <c r="H74" s="2">
+      <c r="H74" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>72</v>
       </c>
-      <c r="C75" s="2">
+      <c r="C75" s="1">
         <v>22</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="1">
         <v>11</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F75" s="1">
         <v>72</v>
       </c>
-      <c r="G75" s="2">
+      <c r="G75" s="1">
         <v>14</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>73</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="1">
         <v>21</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76" s="1">
         <v>13</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76" s="1">
         <v>73</v>
       </c>
-      <c r="G76" s="2">
+      <c r="G76" s="1">
         <v>13</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>74</v>
       </c>
-      <c r="C77" s="2">
+      <c r="C77" s="1">
         <v>23</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="1">
         <v>13</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77" s="1">
         <v>74</v>
       </c>
-      <c r="G77" s="2">
+      <c r="G77" s="1">
         <v>13</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>75</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="1">
         <v>23</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78" s="1">
         <v>11</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78" s="1">
         <v>75</v>
       </c>
-      <c r="G78" s="2">
+      <c r="G78" s="1">
         <v>15</v>
       </c>
-      <c r="H78" s="2">
+      <c r="H78" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>76</v>
       </c>
-      <c r="C79" s="2">
+      <c r="C79" s="1">
         <v>23</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79" s="1">
         <v>11</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="1">
         <v>76</v>
       </c>
-      <c r="G79" s="2">
+      <c r="G79" s="1">
         <v>13</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H79" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>77</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="1">
         <v>21</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80" s="1">
         <v>14</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F80" s="1">
         <v>77</v>
       </c>
-      <c r="G80" s="2">
+      <c r="G80" s="1">
         <v>15</v>
       </c>
-      <c r="H80" s="2">
+      <c r="H80" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>78</v>
       </c>
-      <c r="C81" s="2">
+      <c r="C81" s="1">
         <v>23</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81" s="1">
         <v>10</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F81" s="1">
         <v>78</v>
       </c>
-      <c r="G81" s="2">
+      <c r="G81" s="1">
         <v>15</v>
       </c>
-      <c r="H81" s="2">
+      <c r="H81" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>79</v>
       </c>
-      <c r="C82" s="2">
+      <c r="C82" s="1">
         <v>22</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82" s="1">
         <v>13</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82" s="1">
         <v>79</v>
       </c>
-      <c r="G82" s="2">
+      <c r="G82" s="1">
         <v>15</v>
       </c>
-      <c r="H82" s="2">
+      <c r="H82" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>80</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="1">
         <v>21</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83" s="1">
         <v>13</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83" s="1">
         <v>80</v>
       </c>
-      <c r="G83" s="2">
+      <c r="G83" s="1">
         <v>13</v>
       </c>
-      <c r="H83" s="2">
+      <c r="H83" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>81</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="1">
         <v>22</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84" s="1">
         <v>11</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F84" s="1">
         <v>81</v>
       </c>
-      <c r="G84" s="2">
+      <c r="G84" s="1">
         <v>13</v>
       </c>
-      <c r="H84" s="2">
+      <c r="H84" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>82</v>
       </c>
-      <c r="C85" s="2">
+      <c r="C85" s="1">
         <v>21</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85" s="1">
         <v>11</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F85" s="1">
         <v>82</v>
       </c>
-      <c r="G85" s="2">
+      <c r="G85" s="1">
         <v>15</v>
       </c>
-      <c r="H85" s="2">
+      <c r="H85" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>83</v>
       </c>
-      <c r="C86" s="2">
+      <c r="C86" s="1">
         <v>23</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86" s="1">
         <v>12</v>
       </c>
-      <c r="F86" s="2">
+      <c r="F86" s="1">
         <v>83</v>
       </c>
-      <c r="G86" s="2">
+      <c r="G86" s="1">
         <v>15</v>
       </c>
-      <c r="H86" s="2">
+      <c r="H86" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>84</v>
       </c>
-      <c r="C87" s="2">
+      <c r="C87" s="1">
         <v>21</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87" s="1">
         <v>13</v>
       </c>
-      <c r="F87" s="2">
+      <c r="F87" s="1">
         <v>84</v>
       </c>
-      <c r="G87" s="2">
+      <c r="G87" s="1">
         <v>13</v>
       </c>
-      <c r="H87" s="2">
+      <c r="H87" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>85</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C88" s="1">
         <v>22</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88" s="1">
         <v>10</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F88" s="1">
         <v>85</v>
       </c>
-      <c r="G88" s="2">
+      <c r="G88" s="1">
         <v>13</v>
       </c>
-      <c r="H88" s="2">
+      <c r="H88" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>86</v>
       </c>
-      <c r="C89" s="2">
+      <c r="C89" s="1">
         <v>21</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89" s="1">
         <v>13</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F89" s="1">
         <v>86</v>
       </c>
-      <c r="G89" s="2">
+      <c r="G89" s="1">
         <v>15</v>
       </c>
-      <c r="H89" s="2">
+      <c r="H89" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>87</v>
       </c>
-      <c r="C90" s="2">
+      <c r="C90" s="1">
         <v>21</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90" s="1">
         <v>11</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F90" s="1">
         <v>87</v>
       </c>
-      <c r="G90" s="2">
+      <c r="G90" s="1">
         <v>14</v>
       </c>
-      <c r="H90" s="2">
+      <c r="H90" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>88</v>
       </c>
-      <c r="C91" s="2">
+      <c r="C91" s="1">
         <v>23</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91" s="1">
         <v>11</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91" s="1">
         <v>88</v>
       </c>
-      <c r="G91" s="2">
+      <c r="G91" s="1">
         <v>15</v>
       </c>
-      <c r="H91" s="2">
+      <c r="H91" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>89</v>
       </c>
-      <c r="C92" s="2">
+      <c r="C92" s="1">
         <v>21</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="1">
         <v>12</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F92" s="1">
         <v>89</v>
       </c>
-      <c r="G92" s="2">
+      <c r="G92" s="1">
         <v>15</v>
       </c>
-      <c r="H92" s="2">
+      <c r="H92" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>90</v>
       </c>
-      <c r="C93" s="2">
+      <c r="C93" s="1">
         <v>22</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93" s="1">
         <v>14</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F93" s="1">
         <v>90</v>
       </c>
-      <c r="G93" s="2">
+      <c r="G93" s="1">
         <v>15</v>
       </c>
-      <c r="H93" s="2">
+      <c r="H93" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>91</v>
       </c>
-      <c r="C94" s="2">
+      <c r="C94" s="1">
         <v>23</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94" s="1">
         <v>14</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F94" s="1">
         <v>91</v>
       </c>
-      <c r="G94" s="2">
+      <c r="G94" s="1">
         <v>14</v>
       </c>
-      <c r="H94" s="2">
+      <c r="H94" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>92</v>
       </c>
-      <c r="C95" s="2">
+      <c r="C95" s="1">
         <v>21</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D95" s="1">
         <v>12</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95" s="1">
         <v>92</v>
       </c>
-      <c r="G95" s="2">
+      <c r="G95" s="1">
         <v>15</v>
       </c>
-      <c r="H95" s="2">
+      <c r="H95" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>93</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C96" s="1">
         <v>23</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D96" s="1">
         <v>13</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F96" s="1">
         <v>93</v>
       </c>
-      <c r="G96" s="2">
+      <c r="G96" s="1">
         <v>14</v>
       </c>
-      <c r="H96" s="2">
+      <c r="H96" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B97" s="2">
+      <c r="B97" s="1">
         <v>94</v>
       </c>
-      <c r="C97" s="2">
+      <c r="C97" s="1">
         <v>22</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97" s="1">
         <v>14</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F97" s="1">
         <v>94</v>
       </c>
-      <c r="G97" s="2">
+      <c r="G97" s="1">
         <v>14</v>
       </c>
-      <c r="H97" s="2">
+      <c r="H97" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>95</v>
       </c>
-      <c r="C98" s="2">
+      <c r="C98" s="1">
         <v>22</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D98" s="1">
         <v>10</v>
       </c>
-      <c r="F98" s="2">
+      <c r="F98" s="1">
         <v>95</v>
       </c>
-      <c r="G98" s="2">
+      <c r="G98" s="1">
         <v>13</v>
       </c>
-      <c r="H98" s="2">
+      <c r="H98" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>96</v>
       </c>
-      <c r="C99" s="2">
+      <c r="C99" s="1">
         <v>22</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99" s="1">
         <v>10</v>
       </c>
-      <c r="F99" s="2">
+      <c r="F99" s="1">
         <v>96</v>
       </c>
-      <c r="G99" s="2">
+      <c r="G99" s="1">
         <v>15</v>
       </c>
-      <c r="H99" s="2">
+      <c r="H99" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>97</v>
       </c>
-      <c r="C100" s="2">
+      <c r="C100" s="1">
         <v>21</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100" s="1">
         <v>12</v>
       </c>
-      <c r="F100" s="2">
+      <c r="F100" s="1">
         <v>97</v>
       </c>
-      <c r="G100" s="2">
+      <c r="G100" s="1">
         <v>15</v>
       </c>
-      <c r="H100" s="2">
+      <c r="H100" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B101" s="2">
+      <c r="B101" s="1">
         <v>98</v>
       </c>
-      <c r="C101" s="2">
+      <c r="C101" s="1">
         <v>23</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101" s="1">
         <v>13</v>
       </c>
-      <c r="F101" s="2">
+      <c r="F101" s="1">
         <v>98</v>
       </c>
-      <c r="G101" s="2">
+      <c r="G101" s="1">
         <v>13</v>
       </c>
-      <c r="H101" s="2">
+      <c r="H101" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B102" s="2">
+      <c r="B102" s="1">
         <v>99</v>
       </c>
-      <c r="C102" s="2">
+      <c r="C102" s="1">
         <v>21</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102" s="1">
         <v>12</v>
       </c>
-      <c r="F102" s="2">
+      <c r="F102" s="1">
         <v>99</v>
       </c>
-      <c r="G102" s="2">
+      <c r="G102" s="1">
         <v>15</v>
       </c>
-      <c r="H102" s="2">
+      <c r="H102" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B103" s="2">
+      <c r="B103" s="1">
         <v>100</v>
       </c>
-      <c r="C103" s="2">
+      <c r="C103" s="1">
         <v>21</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D103" s="1">
         <v>10</v>
       </c>
-      <c r="F103" s="2">
+      <c r="F103" s="1">
         <v>100</v>
       </c>
-      <c r="G103" s="2">
+      <c r="G103" s="1">
         <v>13</v>
       </c>
-      <c r="H103" s="2">
+      <c r="H103" s="1">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
opt2_3: add auxiliary windows management and make slight code improvements
</commit_message>
<xml_diff>
--- a/misc/opt1.xlsx
+++ b/misc/opt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanshtarev/Documents/Work/repos/rubik_solver/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62694EAA-F212-EE45-8469-8C141DAC4A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C29352-7EC7-B147-9C60-BFACBE4D7387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38540" yWindow="-240" windowWidth="40800" windowHeight="25380" xr2:uid="{EAAB80E9-7C5A-234D-BF3F-DF62DD458500}"/>
+    <workbookView xWindow="-20" yWindow="900" windowWidth="41120" windowHeight="24460" xr2:uid="{EAAB80E9-7C5A-234D-BF3F-DF62DD458500}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Main Window, ms</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>Buffers Optimization</t>
+  </si>
+  <si>
+    <t>Speed Increase</t>
+  </si>
+  <si>
+    <t>Main Window, %</t>
+  </si>
+  <si>
+    <t>Input Window, %</t>
   </si>
 </sst>
 </file>
@@ -124,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -136,6 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4757,16 +4767,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>726439</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>20320</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>405289</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>107907</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>100792</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>801481</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>138387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4793,16 +4803,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>421144</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>132109</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>72853</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>17780</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>817336</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>163758</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5129,10 +5139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D7FD23-B911-0D40-9577-06D9A79B11E5}">
-  <dimension ref="B2:H103"/>
+  <dimension ref="B2:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I27" zoomScale="125" workbookViewId="0">
-      <selection activeCell="P71" sqref="P71"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5144,9 +5154,11 @@
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="15.83203125" customWidth="1"/>
     <col min="9" max="9" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -5157,8 +5169,12 @@
         <v>3</v>
       </c>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -5173,8 +5189,14 @@
       <c r="H3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -5193,8 +5215,16 @@
       <c r="H4" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J4" s="5">
+        <f>(C4-G4)/C4</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K4" s="5">
+        <f>(D4-H4)/D4</f>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -5213,8 +5243,16 @@
       <c r="H5" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J5" s="5">
+        <f t="shared" ref="J5:K68" si="0">(C5-G5)/C5</f>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -5233,8 +5271,16 @@
       <c r="H6" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -5253,8 +5299,16 @@
       <c r="H7" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -5273,8 +5327,16 @@
       <c r="H8" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -5293,8 +5355,16 @@
       <c r="H9" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -5313,8 +5383,16 @@
       <c r="H10" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -5333,8 +5411,16 @@
       <c r="H11" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>9</v>
       </c>
@@ -5353,8 +5439,16 @@
       <c r="H12" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -5373,8 +5467,16 @@
       <c r="H13" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>11</v>
       </c>
@@ -5393,8 +5495,16 @@
       <c r="H14" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>12</v>
       </c>
@@ -5413,8 +5523,16 @@
       <c r="H15" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>13</v>
       </c>
@@ -5433,8 +5551,16 @@
       <c r="H16" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -5453,8 +5579,16 @@
       <c r="H17" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>15</v>
       </c>
@@ -5473,8 +5607,16 @@
       <c r="H18" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>16</v>
       </c>
@@ -5493,8 +5635,16 @@
       <c r="H19" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>17</v>
       </c>
@@ -5513,8 +5663,16 @@
       <c r="H20" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>18</v>
       </c>
@@ -5533,8 +5691,16 @@
       <c r="H21" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7857142857142857</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>19</v>
       </c>
@@ -5553,8 +5719,16 @@
       <c r="H22" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>20</v>
       </c>
@@ -5573,8 +5747,16 @@
       <c r="H23" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>21</v>
       </c>
@@ -5593,8 +5775,16 @@
       <c r="H24" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J24" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>22</v>
       </c>
@@ -5613,8 +5803,16 @@
       <c r="H25" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J25" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>23</v>
       </c>
@@ -5633,8 +5831,16 @@
       <c r="H26" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>24</v>
       </c>
@@ -5653,8 +5859,16 @@
       <c r="H27" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>25</v>
       </c>
@@ -5673,8 +5887,16 @@
       <c r="H28" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>26</v>
       </c>
@@ -5693,8 +5915,16 @@
       <c r="H29" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J29" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>27</v>
       </c>
@@ -5713,8 +5943,16 @@
       <c r="H30" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B31" s="1">
         <v>28</v>
       </c>
@@ -5733,8 +5971,16 @@
       <c r="H31" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B32" s="1">
         <v>29</v>
       </c>
@@ -5753,8 +5999,16 @@
       <c r="H32" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J32" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
         <v>30</v>
       </c>
@@ -5773,8 +6027,16 @@
       <c r="H33" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B34" s="1">
         <v>31</v>
       </c>
@@ -5793,8 +6055,16 @@
       <c r="H34" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J34" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1">
         <v>32</v>
       </c>
@@ -5813,8 +6083,16 @@
       <c r="H35" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J35" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="0"/>
+        <v>0.61538461538461542</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1">
         <v>33</v>
       </c>
@@ -5833,8 +6111,16 @@
       <c r="H36" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J36" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1">
         <v>34</v>
       </c>
@@ -5853,8 +6139,16 @@
       <c r="H37" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J37" s="5">
+        <f t="shared" si="0"/>
+        <v>0.23809523809523808</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="1">
         <v>35</v>
       </c>
@@ -5873,8 +6167,16 @@
       <c r="H38" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J38" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="1">
         <v>36</v>
       </c>
@@ -5893,8 +6195,16 @@
       <c r="H39" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J39" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" s="1">
         <v>37</v>
       </c>
@@ -5913,8 +6223,16 @@
       <c r="H40" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J40" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="1">
         <v>38</v>
       </c>
@@ -5933,8 +6251,16 @@
       <c r="H41" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J41" s="5">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="0"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42" s="1">
         <v>39</v>
       </c>
@@ -5953,8 +6279,16 @@
       <c r="H42" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J42" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" s="1">
         <v>40</v>
       </c>
@@ -5973,8 +6307,16 @@
       <c r="H43" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J43" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="1">
         <v>41</v>
       </c>
@@ -5993,8 +6335,16 @@
       <c r="H44" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J44" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="1">
         <v>42</v>
       </c>
@@ -6013,8 +6363,16 @@
       <c r="H45" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J45" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="1">
         <v>43</v>
       </c>
@@ -6033,8 +6391,16 @@
       <c r="H46" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J46" s="5">
+        <f t="shared" si="0"/>
+        <v>0.21052631578947367</v>
+      </c>
+      <c r="K46" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="1">
         <v>44</v>
       </c>
@@ -6053,8 +6419,16 @@
       <c r="H47" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J47" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K47" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="1">
         <v>45</v>
       </c>
@@ -6073,8 +6447,16 @@
       <c r="H48" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J48" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K48" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" s="1">
         <v>46</v>
       </c>
@@ -6093,8 +6475,16 @@
       <c r="H49" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J49" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K49" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
         <v>47</v>
       </c>
@@ -6113,8 +6503,16 @@
       <c r="H50" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J50" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K50" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="1">
         <v>48</v>
       </c>
@@ -6133,8 +6531,16 @@
       <c r="H51" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J51" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K51" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" s="1">
         <v>49</v>
       </c>
@@ -6153,8 +6559,16 @@
       <c r="H52" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J52" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K52" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" s="1">
         <v>50</v>
       </c>
@@ -6173,8 +6587,16 @@
       <c r="H53" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J53" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K53" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
         <v>51</v>
       </c>
@@ -6193,8 +6615,16 @@
       <c r="H54" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J54" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K54" s="5">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="1">
         <v>52</v>
       </c>
@@ -6213,8 +6643,16 @@
       <c r="H55" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J55" s="5">
+        <f t="shared" si="0"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K55" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7857142857142857</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B56" s="1">
         <v>53</v>
       </c>
@@ -6233,8 +6671,16 @@
       <c r="H56" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J56" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K56" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B57" s="1">
         <v>54</v>
       </c>
@@ -6253,8 +6699,16 @@
       <c r="H57" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J57" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K57" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B58" s="1">
         <v>55</v>
       </c>
@@ -6273,8 +6727,16 @@
       <c r="H58" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J58" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K58" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B59" s="1">
         <v>56</v>
       </c>
@@ -6293,8 +6755,16 @@
       <c r="H59" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J59" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K59" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B60" s="1">
         <v>57</v>
       </c>
@@ -6313,8 +6783,16 @@
       <c r="H60" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J60" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K60" s="5">
+        <f t="shared" si="0"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B61" s="1">
         <v>58</v>
       </c>
@@ -6333,8 +6811,16 @@
       <c r="H61" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J61" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K61" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B62" s="1">
         <v>59</v>
       </c>
@@ -6353,8 +6839,16 @@
       <c r="H62" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J62" s="5">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K62" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B63" s="1">
         <v>60</v>
       </c>
@@ -6373,8 +6867,16 @@
       <c r="H63" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J63" s="5">
+        <f t="shared" si="0"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K63" s="5">
+        <f t="shared" si="0"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B64" s="1">
         <v>61</v>
       </c>
@@ -6393,8 +6895,16 @@
       <c r="H64" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J64" s="5">
+        <f t="shared" si="0"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K64" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B65" s="1">
         <v>62</v>
       </c>
@@ -6413,8 +6923,16 @@
       <c r="H65" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J65" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K65" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <v>63</v>
       </c>
@@ -6433,8 +6951,16 @@
       <c r="H66" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J66" s="5">
+        <f t="shared" si="0"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K66" s="5">
+        <f t="shared" si="0"/>
+        <v>0.54545454545454541</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B67" s="1">
         <v>64</v>
       </c>
@@ -6453,8 +6979,16 @@
       <c r="H67" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J67" s="5">
+        <f t="shared" si="0"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K67" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B68" s="1">
         <v>65</v>
       </c>
@@ -6473,8 +7007,16 @@
       <c r="H68" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J68" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K68" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="1">
         <v>66</v>
       </c>
@@ -6493,8 +7035,16 @@
       <c r="H69" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J69" s="5">
+        <f t="shared" ref="J69:K103" si="1">(C69-G69)/C69</f>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K69" s="5">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B70" s="1">
         <v>67</v>
       </c>
@@ -6513,8 +7063,16 @@
       <c r="H70" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J70" s="5">
+        <f t="shared" si="1"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K70" s="5">
+        <f t="shared" si="1"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B71" s="1">
         <v>68</v>
       </c>
@@ -6533,8 +7091,16 @@
       <c r="H71" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J71" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K71" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B72" s="1">
         <v>69</v>
       </c>
@@ -6553,8 +7119,16 @@
       <c r="H72" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J72" s="5">
+        <f t="shared" si="1"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K72" s="5">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="1">
         <v>70</v>
       </c>
@@ -6573,8 +7147,16 @@
       <c r="H73" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J73" s="5">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K73" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B74" s="1">
         <v>71</v>
       </c>
@@ -6593,8 +7175,16 @@
       <c r="H74" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J74" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K74" s="5">
+        <f t="shared" si="1"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="1">
         <v>72</v>
       </c>
@@ -6613,8 +7203,16 @@
       <c r="H75" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J75" s="5">
+        <f t="shared" si="1"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K75" s="5">
+        <f t="shared" si="1"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B76" s="1">
         <v>73</v>
       </c>
@@ -6633,8 +7231,16 @@
       <c r="H76" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J76" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K76" s="5">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B77" s="1">
         <v>74</v>
       </c>
@@ -6653,8 +7259,16 @@
       <c r="H77" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J77" s="5">
+        <f t="shared" si="1"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K77" s="5">
+        <f t="shared" si="1"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B78" s="1">
         <v>75</v>
       </c>
@@ -6673,8 +7287,16 @@
       <c r="H78" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J78" s="5">
+        <f t="shared" si="1"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K78" s="5">
+        <f t="shared" si="1"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B79" s="1">
         <v>76</v>
       </c>
@@ -6693,8 +7315,16 @@
       <c r="H79" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J79" s="5">
+        <f t="shared" si="1"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K79" s="5">
+        <f t="shared" si="1"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B80" s="1">
         <v>77</v>
       </c>
@@ -6713,8 +7343,16 @@
       <c r="H80" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J80" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K80" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7857142857142857</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B81" s="1">
         <v>78</v>
       </c>
@@ -6733,8 +7371,16 @@
       <c r="H81" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J81" s="5">
+        <f t="shared" si="1"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K81" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="1">
         <v>79</v>
       </c>
@@ -6753,8 +7399,16 @@
       <c r="H82" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J82" s="5">
+        <f t="shared" si="1"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K82" s="5">
+        <f t="shared" si="1"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="1">
         <v>80</v>
       </c>
@@ -6773,8 +7427,16 @@
       <c r="H83" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J83" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K83" s="5">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="1">
         <v>81</v>
       </c>
@@ -6793,8 +7455,16 @@
       <c r="H84" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J84" s="5">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K84" s="5">
+        <f t="shared" si="1"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="1">
         <v>82</v>
       </c>
@@ -6813,8 +7483,16 @@
       <c r="H85" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J85" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K85" s="5">
+        <f t="shared" si="1"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="1">
         <v>83</v>
       </c>
@@ -6833,8 +7511,16 @@
       <c r="H86" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J86" s="5">
+        <f t="shared" si="1"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K86" s="5">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="1">
         <v>84</v>
       </c>
@@ -6853,8 +7539,16 @@
       <c r="H87" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J87" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K87" s="5">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B88" s="1">
         <v>85</v>
       </c>
@@ -6873,8 +7567,16 @@
       <c r="H88" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J88" s="5">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K88" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B89" s="1">
         <v>86</v>
       </c>
@@ -6893,8 +7595,16 @@
       <c r="H89" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J89" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K89" s="5">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B90" s="1">
         <v>87</v>
       </c>
@@ -6913,8 +7623,16 @@
       <c r="H90" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J90" s="5">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K90" s="5">
+        <f t="shared" si="1"/>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B91" s="1">
         <v>88</v>
       </c>
@@ -6933,8 +7651,16 @@
       <c r="H91" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J91" s="5">
+        <f t="shared" si="1"/>
+        <v>0.34782608695652173</v>
+      </c>
+      <c r="K91" s="5">
+        <f t="shared" si="1"/>
+        <v>0.63636363636363635</v>
+      </c>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B92" s="1">
         <v>89</v>
       </c>
@@ -6953,8 +7679,16 @@
       <c r="H92" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J92" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K92" s="5">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B93" s="1">
         <v>90</v>
       </c>
@@ -6973,8 +7707,16 @@
       <c r="H93" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J93" s="5">
+        <f t="shared" si="1"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K93" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B94" s="1">
         <v>91</v>
       </c>
@@ -6993,8 +7735,16 @@
       <c r="H94" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J94" s="5">
+        <f t="shared" si="1"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K94" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7857142857142857</v>
+      </c>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B95" s="1">
         <v>92</v>
       </c>
@@ -7013,8 +7763,16 @@
       <c r="H95" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J95" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K95" s="5">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B96" s="1">
         <v>93</v>
       </c>
@@ -7033,8 +7791,16 @@
       <c r="H96" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J96" s="5">
+        <f t="shared" si="1"/>
+        <v>0.39130434782608697</v>
+      </c>
+      <c r="K96" s="5">
+        <f t="shared" si="1"/>
+        <v>0.69230769230769229</v>
+      </c>
+    </row>
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B97" s="1">
         <v>94</v>
       </c>
@@ -7053,8 +7819,16 @@
       <c r="H97" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J97" s="5">
+        <f t="shared" si="1"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K97" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7857142857142857</v>
+      </c>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B98" s="1">
         <v>95</v>
       </c>
@@ -7073,8 +7847,16 @@
       <c r="H98" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J98" s="5">
+        <f t="shared" si="1"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="K98" s="5">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B99" s="1">
         <v>96</v>
       </c>
@@ -7093,8 +7875,16 @@
       <c r="H99" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J99" s="5">
+        <f t="shared" si="1"/>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="K99" s="5">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B100" s="1">
         <v>97</v>
       </c>
@@ -7113,8 +7903,16 @@
       <c r="H100" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J100" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K100" s="5">
+        <f t="shared" si="1"/>
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="101" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B101" s="1">
         <v>98</v>
       </c>
@@ -7133,8 +7931,16 @@
       <c r="H101" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J101" s="5">
+        <f t="shared" si="1"/>
+        <v>0.43478260869565216</v>
+      </c>
+      <c r="K101" s="5">
+        <f t="shared" si="1"/>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="102" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B102" s="1">
         <v>99</v>
       </c>
@@ -7153,8 +7959,16 @@
       <c r="H102" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="J102" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="K102" s="5">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B103" s="1">
         <v>100</v>
       </c>
@@ -7173,11 +7987,30 @@
       <c r="H103" s="1">
         <v>4</v>
       </c>
+      <c r="J103" s="5">
+        <f t="shared" si="1"/>
+        <v>0.38095238095238093</v>
+      </c>
+      <c r="K103" s="5">
+        <f t="shared" si="1"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J105" s="5">
+        <f>AVERAGE(J4:J103)</f>
+        <v>0.35469918373007592</v>
+      </c>
+      <c r="K105" s="5">
+        <f>AVERAGE(K4:K103)</f>
+        <v>0.6975098235098236</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C2:D2"/>
+    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
measure opt4 data and update opt1 graphs
</commit_message>
<xml_diff>
--- a/misc/opt1.xlsx
+++ b/misc/opt1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanshtarev/Documents/Work/repos/rubik_solver/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041045FA-C3BD-A344-935A-DF58072356BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68032FB-8706-FD4C-810B-F469DA05D41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19860" xr2:uid="{EAAB80E9-7C5A-234D-BF3F-DF62DD458500}"/>
+    <workbookView xWindow="38520" yWindow="-260" windowWidth="40800" windowHeight="25380" xr2:uid="{EAAB80E9-7C5A-234D-BF3F-DF62DD458500}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Main Window, ms</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Speed Increase, -Ofast</t>
+  </si>
+  <si>
+    <t>Speed Increase, no -Ofast</t>
   </si>
 </sst>
 </file>
@@ -909,15 +912,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Buffers Optimization, -Ofast</c:v>
+                  <c:v>Buffers Optimization, no -Ofast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -948,7 +951,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$103</c:f>
+              <c:f>Sheet1!$J$4:$J$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1257,309 +1260,309 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$103</c:f>
+              <c:f>Sheet1!$K$4:$K$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="33">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="41">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="34">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>14</c:v>
-                </c:pt>
                 <c:pt idx="42">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>13</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>13</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>13</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>15</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1567,20 +1570,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-2536-1A48-8FBA-FDCA35515254}"/>
+              <c16:uniqueId val="{00000000-E747-AC4C-BFF0-843E760E973E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$2</c:f>
+              <c:f>Sheet1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Buffers Optimization, no -Ofast</c:v>
+                  <c:v>Buffers Optimization, -Ofast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1611,7 +1614,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$4:$J$103</c:f>
+              <c:f>Sheet1!$F$4:$F$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1920,309 +1923,309 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$103</c:f>
+              <c:f>Sheet1!$G$4:$G$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>17</c:v>
-                </c:pt>
                 <c:pt idx="34">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>18</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>18</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>19</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>17</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>18</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>17</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>19</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>19</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>18</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2230,7 +2233,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E747-AC4C-BFF0-843E760E973E}"/>
+              <c16:uniqueId val="{00000001-2536-1A48-8FBA-FDCA35515254}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2289,7 +2292,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2000"/>
-                  <a:t>Frame</a:t>
+                  <a:t>Frame No.</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2346,7 +2349,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2470,7 +2473,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3315,15 +3318,15 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>Sheet1!$K$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Buffers Optimization, -Ofast</c:v>
+                  <c:v>Buffers Optimization, no -Ofast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3354,7 +3357,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$103</c:f>
+              <c:f>Sheet1!$J$4:$J$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -3663,309 +3666,309 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$4:$H$103</c:f>
+              <c:f>Sheet1!$L$4:$L$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>3</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3973,20 +3976,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-106A-984B-8AD5-7B46BC777B6B}"/>
+              <c16:uniqueId val="{00000000-00F6-054C-B3AC-8B1685E40EEF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$2</c:f>
+              <c:f>Sheet1!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Buffers Optimization, no -Ofast</c:v>
+                  <c:v>Buffers Optimization, -Ofast</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4017,7 +4020,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$J$4:$J$103</c:f>
+              <c:f>Sheet1!$F$4:$F$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -4326,309 +4329,309 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$103</c:f>
+              <c:f>Sheet1!$H$4:$H$103</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4636,7 +4639,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-00F6-054C-B3AC-8B1685E40EEF}"/>
+              <c16:uniqueId val="{00000001-106A-984B-8AD5-7B46BC777B6B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4695,7 +4698,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2000"/>
-                  <a:t>Frame</a:t>
+                  <a:t> Frame No.</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4752,7 +4755,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4877,7 +4880,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6102,10 +6105,10 @@
       <xdr:rowOff>53283</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>364492</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>83763</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>220869</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>73623</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6133,15 +6136,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>791805</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>50173</xdr:rowOff>
+      <xdr:colOff>810211</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>68578</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>361489</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>81822</xdr:rowOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>202463</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>18406</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6470,8 +6473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8D7FD23-B911-0D40-9577-06D9A79B11E5}">
   <dimension ref="B2:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="AT26" sqref="AT26"/>
+    <sheetView tabSelected="1" topLeftCell="R32" workbookViewId="0">
+      <selection activeCell="AV71" sqref="AV71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6513,7 +6516,7 @@
       </c>
       <c r="O2" s="3"/>
       <c r="Q2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="R2" s="3"/>
     </row>
@@ -6581,11 +6584,11 @@
         <v>8</v>
       </c>
       <c r="N4" s="2">
-        <f>(C4-G4)/C4</f>
+        <f t="shared" ref="N4:N35" si="0">(C4-G4)/C4</f>
         <v>0.36363636363636365</v>
       </c>
       <c r="O4" s="2">
-        <f>(D4-H4)/D4</f>
+        <f t="shared" ref="O4:O35" si="1">(D4-H4)/D4</f>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q4" s="2">
@@ -6626,19 +6629,19 @@
         <v>9</v>
       </c>
       <c r="N5" s="2">
-        <f>(C5-G5)/C5</f>
+        <f t="shared" si="0"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O5" s="2">
-        <f>(D5-H5)/D5</f>
+        <f t="shared" si="1"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q5" s="2">
-        <f t="shared" ref="Q5:Q68" si="0">(C5-K5)/C5</f>
+        <f t="shared" ref="Q5:Q68" si="2">(C5-K5)/C5</f>
         <v>0.21739130434782608</v>
       </c>
       <c r="R5" s="2">
-        <f t="shared" ref="R5:R68" si="1">(D5-L5)/D5</f>
+        <f t="shared" ref="R5:R68" si="3">(D5-L5)/D5</f>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -6671,19 +6674,19 @@
         <v>8</v>
       </c>
       <c r="N6" s="2">
-        <f>(C6-G6)/C6</f>
+        <f t="shared" si="0"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O6" s="2">
-        <f>(D6-H6)/D6</f>
+        <f t="shared" si="1"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -6716,19 +6719,19 @@
         <v>7</v>
       </c>
       <c r="N7" s="2">
-        <f>(C7-G7)/C7</f>
+        <f t="shared" si="0"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O7" s="2">
-        <f>(D7-H7)/D7</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -6761,19 +6764,19 @@
         <v>8</v>
       </c>
       <c r="N8" s="2">
-        <f>(C8-G8)/C8</f>
+        <f t="shared" si="0"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O8" s="2">
-        <f>(D8-H8)/D8</f>
+        <f t="shared" si="1"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="R8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -6806,19 +6809,19 @@
         <v>9</v>
       </c>
       <c r="N9" s="2">
-        <f>(C9-G9)/C9</f>
+        <f t="shared" si="0"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O9" s="2">
-        <f>(D9-H9)/D9</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="R9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
     </row>
@@ -6851,19 +6854,19 @@
         <v>9</v>
       </c>
       <c r="N10" s="2">
-        <f>(C10-G10)/C10</f>
+        <f t="shared" si="0"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O10" s="2">
-        <f>(D10-H10)/D10</f>
+        <f t="shared" si="1"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="R10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -6896,19 +6899,19 @@
         <v>9</v>
       </c>
       <c r="N11" s="2">
-        <f>(C11-G11)/C11</f>
+        <f t="shared" si="0"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O11" s="2">
-        <f>(D11-H11)/D11</f>
+        <f t="shared" si="1"/>
         <v>0.6428571428571429</v>
       </c>
       <c r="Q11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -6941,19 +6944,19 @@
         <v>8</v>
       </c>
       <c r="N12" s="2">
-        <f>(C12-G12)/C12</f>
+        <f t="shared" si="0"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O12" s="2">
-        <f>(D12-H12)/D12</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
       <c r="R12" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -6986,19 +6989,19 @@
         <v>7</v>
       </c>
       <c r="N13" s="2">
-        <f>(C13-G13)/C13</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O13" s="2">
-        <f>(D13-H13)/D13</f>
+        <f t="shared" si="1"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="R13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.46153846153846156</v>
       </c>
     </row>
@@ -7031,19 +7034,19 @@
         <v>9</v>
       </c>
       <c r="N14" s="2">
-        <f>(C14-G14)/C14</f>
+        <f t="shared" si="0"/>
         <v>0.41666666666666669</v>
       </c>
       <c r="O14" s="2">
-        <f>(D14-H14)/D14</f>
+        <f t="shared" si="1"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.20833333333333334</v>
       </c>
       <c r="R14" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -7076,19 +7079,19 @@
         <v>9</v>
       </c>
       <c r="N15" s="2">
-        <f>(C15-G15)/C15</f>
+        <f t="shared" si="0"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O15" s="2">
-        <f>(D15-H15)/D15</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2608695652173913</v>
       </c>
       <c r="R15" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
     </row>
@@ -7121,19 +7124,19 @@
         <v>8</v>
       </c>
       <c r="N16" s="2">
-        <f>(C16-G16)/C16</f>
+        <f t="shared" si="0"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O16" s="2">
-        <f>(D16-H16)/D16</f>
+        <f t="shared" si="1"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R16" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -7166,19 +7169,19 @@
         <v>9</v>
       </c>
       <c r="N17" s="2">
-        <f>(C17-G17)/C17</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O17" s="2">
-        <f>(D17-H17)/D17</f>
+        <f t="shared" si="1"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -7211,19 +7214,19 @@
         <v>8</v>
       </c>
       <c r="N18" s="2">
-        <f>(C18-G18)/C18</f>
+        <f t="shared" si="0"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O18" s="2">
-        <f>(D18-H18)/D18</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="R18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
@@ -7256,19 +7259,19 @@
         <v>9</v>
       </c>
       <c r="N19" s="2">
-        <f>(C19-G19)/C19</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O19" s="2">
-        <f>(D19-H19)/D19</f>
+        <f t="shared" si="1"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -7301,19 +7304,19 @@
         <v>7</v>
       </c>
       <c r="N20" s="2">
-        <f>(C20-G20)/C20</f>
+        <f t="shared" si="0"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O20" s="2">
-        <f>(D20-H20)/D20</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -7346,19 +7349,19 @@
         <v>9</v>
       </c>
       <c r="N21" s="2">
-        <f>(C21-G21)/C21</f>
+        <f t="shared" si="0"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O21" s="2">
-        <f>(D21-H21)/D21</f>
+        <f t="shared" si="1"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -7391,19 +7394,19 @@
         <v>7</v>
       </c>
       <c r="N22" s="2">
-        <f>(C22-G22)/C22</f>
+        <f t="shared" si="0"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O22" s="2">
-        <f>(D22-H22)/D22</f>
+        <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -7436,19 +7439,19 @@
         <v>9</v>
       </c>
       <c r="N23" s="2">
-        <f>(C23-G23)/C23</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O23" s="2">
-        <f>(D23-H23)/D23</f>
+        <f t="shared" si="1"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R23" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -7481,19 +7484,19 @@
         <v>8</v>
       </c>
       <c r="N24" s="2">
-        <f>(C24-G24)/C24</f>
+        <f t="shared" si="0"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O24" s="2">
-        <f>(D24-H24)/D24</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -7526,19 +7529,19 @@
         <v>8</v>
       </c>
       <c r="N25" s="2">
-        <f>(C25-G25)/C25</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O25" s="2">
-        <f>(D25-H25)/D25</f>
+        <f t="shared" si="1"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q25" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R25" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -7571,19 +7574,19 @@
         <v>8</v>
       </c>
       <c r="N26" s="2">
-        <f>(C26-G26)/C26</f>
+        <f t="shared" si="0"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O26" s="2">
-        <f>(D26-H26)/D26</f>
+        <f t="shared" si="1"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q26" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -7616,19 +7619,19 @@
         <v>9</v>
       </c>
       <c r="N27" s="2">
-        <f>(C27-G27)/C27</f>
+        <f t="shared" si="0"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O27" s="2">
-        <f>(D27-H27)/D27</f>
+        <f t="shared" si="1"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.21739130434782608</v>
       </c>
       <c r="R27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -7661,19 +7664,19 @@
         <v>9</v>
       </c>
       <c r="N28" s="2">
-        <f>(C28-G28)/C28</f>
+        <f t="shared" si="0"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O28" s="2">
-        <f>(D28-H28)/D28</f>
+        <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
       <c r="Q28" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
     </row>
@@ -7706,19 +7709,19 @@
         <v>8</v>
       </c>
       <c r="N29" s="2">
-        <f>(C29-G29)/C29</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O29" s="2">
-        <f>(D29-H29)/D29</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="Q29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="R29" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
@@ -7751,19 +7754,19 @@
         <v>7</v>
       </c>
       <c r="N30" s="2">
-        <f>(C30-G30)/C30</f>
+        <f t="shared" si="0"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O30" s="2">
-        <f>(D30-H30)/D30</f>
+        <f t="shared" si="1"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q30" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R30" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.36363636363636365</v>
       </c>
     </row>
@@ -7796,19 +7799,19 @@
         <v>8</v>
       </c>
       <c r="N31" s="2">
-        <f>(C31-G31)/C31</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O31" s="2">
-        <f>(D31-H31)/D31</f>
+        <f t="shared" si="1"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q31" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R31" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.27272727272727271</v>
       </c>
     </row>
@@ -7841,19 +7844,19 @@
         <v>8</v>
       </c>
       <c r="N32" s="2">
-        <f>(C32-G32)/C32</f>
+        <f t="shared" si="0"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O32" s="2">
-        <f>(D32-H32)/D32</f>
+        <f t="shared" si="1"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R32" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -7886,19 +7889,19 @@
         <v>8</v>
       </c>
       <c r="N33" s="2">
-        <f>(C33-G33)/C33</f>
+        <f t="shared" si="0"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O33" s="2">
-        <f>(D33-H33)/D33</f>
+        <f t="shared" si="1"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="R33" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -7931,19 +7934,19 @@
         <v>7</v>
       </c>
       <c r="N34" s="2">
-        <f>(C34-G34)/C34</f>
+        <f t="shared" si="0"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O34" s="2">
-        <f>(D34-H34)/D34</f>
+        <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
       <c r="Q34" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R34" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -7976,19 +7979,19 @@
         <v>9</v>
       </c>
       <c r="N35" s="2">
-        <f>(C35-G35)/C35</f>
+        <f t="shared" si="0"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O35" s="2">
-        <f>(D35-H35)/D35</f>
+        <f t="shared" si="1"/>
         <v>0.61538461538461542</v>
       </c>
       <c r="Q35" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R35" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -8021,19 +8024,19 @@
         <v>9</v>
       </c>
       <c r="N36" s="2">
-        <f>(C36-G36)/C36</f>
+        <f t="shared" ref="N36:N67" si="4">(C36-G36)/C36</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="O36" s="2">
-        <f>(D36-H36)/D36</f>
+        <f t="shared" ref="O36:O67" si="5">(D36-H36)/D36</f>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q36" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R36" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -8066,19 +8069,19 @@
         <v>9</v>
       </c>
       <c r="N37" s="2">
-        <f>(C37-G37)/C37</f>
+        <f t="shared" si="4"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="O37" s="2">
-        <f>(D37-H37)/D37</f>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q37" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R37" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
     </row>
@@ -8111,19 +8114,19 @@
         <v>7</v>
       </c>
       <c r="N38" s="2">
-        <f>(C38-G38)/C38</f>
+        <f t="shared" si="4"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O38" s="2">
-        <f>(D38-H38)/D38</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="Q38" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="R38" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -8156,19 +8159,19 @@
         <v>9</v>
       </c>
       <c r="N39" s="2">
-        <f>(C39-G39)/C39</f>
+        <f t="shared" si="4"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O39" s="2">
-        <f>(D39-H39)/D39</f>
+        <f t="shared" si="5"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q39" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R39" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -8201,19 +8204,19 @@
         <v>7</v>
       </c>
       <c r="N40" s="2">
-        <f>(C40-G40)/C40</f>
+        <f t="shared" si="4"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O40" s="2">
-        <f>(D40-H40)/D40</f>
+        <f t="shared" si="5"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q40" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2608695652173913</v>
       </c>
       <c r="R40" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.36363636363636365</v>
       </c>
     </row>
@@ -8246,19 +8249,19 @@
         <v>9</v>
       </c>
       <c r="N41" s="2">
-        <f>(C41-G41)/C41</f>
+        <f t="shared" si="4"/>
         <v>0.3</v>
       </c>
       <c r="O41" s="2">
-        <f>(D41-H41)/D41</f>
+        <f t="shared" si="5"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q41" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
       <c r="R41" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -8291,19 +8294,19 @@
         <v>9</v>
       </c>
       <c r="N42" s="2">
-        <f>(C42-G42)/C42</f>
+        <f t="shared" si="4"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O42" s="2">
-        <f>(D42-H42)/D42</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="Q42" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R42" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
@@ -8336,19 +8339,19 @@
         <v>8</v>
       </c>
       <c r="N43" s="2">
-        <f>(C43-G43)/C43</f>
+        <f t="shared" si="4"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O43" s="2">
-        <f>(D43-H43)/D43</f>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q43" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R43" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -8381,19 +8384,19 @@
         <v>8</v>
       </c>
       <c r="N44" s="2">
-        <f>(C44-G44)/C44</f>
+        <f t="shared" si="4"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O44" s="2">
-        <f>(D44-H44)/D44</f>
+        <f t="shared" si="5"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q44" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R44" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -8426,19 +8429,19 @@
         <v>8</v>
       </c>
       <c r="N45" s="2">
-        <f>(C45-G45)/C45</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O45" s="2">
-        <f>(D45-H45)/D45</f>
+        <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q45" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R45" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -8471,19 +8474,19 @@
         <v>7</v>
       </c>
       <c r="N46" s="2">
-        <f>(C46-G46)/C46</f>
+        <f t="shared" si="4"/>
         <v>0.21052631578947367</v>
       </c>
       <c r="O46" s="2">
-        <f>(D46-H46)/D46</f>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="Q46" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -8516,19 +8519,19 @@
         <v>7</v>
       </c>
       <c r="N47" s="2">
-        <f>(C47-G47)/C47</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O47" s="2">
-        <f>(D47-H47)/D47</f>
+        <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q47" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R47" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.46153846153846156</v>
       </c>
     </row>
@@ -8561,19 +8564,19 @@
         <v>8</v>
       </c>
       <c r="N48" s="2">
-        <f>(C48-G48)/C48</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O48" s="2">
-        <f>(D48-H48)/D48</f>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q48" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R48" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -8606,19 +8609,19 @@
         <v>7</v>
       </c>
       <c r="N49" s="2">
-        <f>(C49-G49)/C49</f>
+        <f t="shared" si="4"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O49" s="2">
-        <f>(D49-H49)/D49</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="Q49" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="R49" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -8651,19 +8654,19 @@
         <v>8</v>
       </c>
       <c r="N50" s="2">
-        <f>(C50-G50)/C50</f>
+        <f t="shared" si="4"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O50" s="2">
-        <f>(D50-H50)/D50</f>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="Q50" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R50" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -8696,19 +8699,19 @@
         <v>8</v>
       </c>
       <c r="N51" s="2">
-        <f>(C51-G51)/C51</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O51" s="2">
-        <f>(D51-H51)/D51</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="Q51" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R51" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
@@ -8741,19 +8744,19 @@
         <v>8</v>
       </c>
       <c r="N52" s="2">
-        <f>(C52-G52)/C52</f>
+        <f t="shared" si="4"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O52" s="2">
-        <f>(D52-H52)/D52</f>
+        <f t="shared" si="5"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q52" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R52" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.27272727272727271</v>
       </c>
     </row>
@@ -8786,19 +8789,19 @@
         <v>9</v>
       </c>
       <c r="N53" s="2">
-        <f>(C53-G53)/C53</f>
+        <f t="shared" si="4"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O53" s="2">
-        <f>(D53-H53)/D53</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="Q53" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R53" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
@@ -8831,19 +8834,19 @@
         <v>8</v>
       </c>
       <c r="N54" s="2">
-        <f>(C54-G54)/C54</f>
+        <f t="shared" si="4"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O54" s="2">
-        <f>(D54-H54)/D54</f>
+        <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
       <c r="Q54" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R54" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -8876,19 +8879,19 @@
         <v>7</v>
       </c>
       <c r="N55" s="2">
-        <f>(C55-G55)/C55</f>
+        <f t="shared" si="4"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O55" s="2">
-        <f>(D55-H55)/D55</f>
+        <f t="shared" si="5"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Q55" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R55" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8921,19 +8924,19 @@
         <v>9</v>
       </c>
       <c r="N56" s="2">
-        <f>(C56-G56)/C56</f>
+        <f t="shared" si="4"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O56" s="2">
-        <f>(D56-H56)/D56</f>
+        <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q56" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R56" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -8966,19 +8969,19 @@
         <v>8</v>
       </c>
       <c r="N57" s="2">
-        <f>(C57-G57)/C57</f>
+        <f t="shared" si="4"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O57" s="2">
-        <f>(D57-H57)/D57</f>
+        <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q57" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R57" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -9011,19 +9014,19 @@
         <v>8</v>
       </c>
       <c r="N58" s="2">
-        <f>(C58-G58)/C58</f>
+        <f t="shared" si="4"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O58" s="2">
-        <f>(D58-H58)/D58</f>
+        <f t="shared" si="5"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q58" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R58" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -9056,19 +9059,19 @@
         <v>9</v>
       </c>
       <c r="N59" s="2">
-        <f>(C59-G59)/C59</f>
+        <f t="shared" si="4"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O59" s="2">
-        <f>(D59-H59)/D59</f>
+        <f t="shared" si="5"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q59" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R59" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -9101,19 +9104,19 @@
         <v>9</v>
       </c>
       <c r="N60" s="2">
-        <f>(C60-G60)/C60</f>
+        <f t="shared" si="4"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O60" s="2">
-        <f>(D60-H60)/D60</f>
+        <f t="shared" si="5"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q60" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R60" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -9146,19 +9149,19 @@
         <v>9</v>
       </c>
       <c r="N61" s="2">
-        <f>(C61-G61)/C61</f>
+        <f t="shared" si="4"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O61" s="2">
-        <f>(D61-H61)/D61</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="Q61" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R61" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
@@ -9191,19 +9194,19 @@
         <v>9</v>
       </c>
       <c r="N62" s="2">
-        <f>(C62-G62)/C62</f>
+        <f t="shared" si="4"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O62" s="2">
-        <f>(D62-H62)/D62</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="Q62" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R62" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
@@ -9236,19 +9239,19 @@
         <v>7</v>
       </c>
       <c r="N63" s="2">
-        <f>(C63-G63)/C63</f>
+        <f t="shared" si="4"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O63" s="2">
-        <f>(D63-H63)/D63</f>
+        <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q63" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R63" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.46153846153846156</v>
       </c>
     </row>
@@ -9281,19 +9284,19 @@
         <v>9</v>
       </c>
       <c r="N64" s="2">
-        <f>(C64-G64)/C64</f>
+        <f t="shared" si="4"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O64" s="2">
-        <f>(D64-H64)/D64</f>
+        <f t="shared" si="5"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q64" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="R64" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -9326,19 +9329,19 @@
         <v>7</v>
       </c>
       <c r="N65" s="2">
-        <f>(C65-G65)/C65</f>
+        <f t="shared" si="4"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O65" s="2">
-        <f>(D65-H65)/D65</f>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="Q65" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R65" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
     </row>
@@ -9371,19 +9374,19 @@
         <v>7</v>
       </c>
       <c r="N66" s="2">
-        <f>(C66-G66)/C66</f>
+        <f t="shared" si="4"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O66" s="2">
-        <f>(D66-H66)/D66</f>
+        <f t="shared" si="5"/>
         <v>0.54545454545454541</v>
       </c>
       <c r="Q66" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2608695652173913</v>
       </c>
       <c r="R66" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.36363636363636365</v>
       </c>
     </row>
@@ -9416,19 +9419,19 @@
         <v>9</v>
       </c>
       <c r="N67" s="2">
-        <f>(C67-G67)/C67</f>
+        <f t="shared" si="4"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O67" s="2">
-        <f>(D67-H67)/D67</f>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
       <c r="Q67" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="R67" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
@@ -9461,19 +9464,19 @@
         <v>8</v>
       </c>
       <c r="N68" s="2">
-        <f>(C68-G68)/C68</f>
+        <f t="shared" ref="N68:N103" si="6">(C68-G68)/C68</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="O68" s="2">
-        <f>(D68-H68)/D68</f>
+        <f t="shared" ref="O68:O103" si="7">(D68-H68)/D68</f>
         <v>0.6</v>
       </c>
       <c r="Q68" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R68" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
@@ -9506,19 +9509,19 @@
         <v>9</v>
       </c>
       <c r="N69" s="2">
-        <f>(C69-G69)/C69</f>
+        <f t="shared" si="6"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O69" s="2">
-        <f>(D69-H69)/D69</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="Q69" s="2">
-        <f t="shared" ref="Q69:Q103" si="2">(C69-K69)/C69</f>
+        <f t="shared" ref="Q69:Q103" si="8">(C69-K69)/C69</f>
         <v>0.17391304347826086</v>
       </c>
       <c r="R69" s="2">
-        <f t="shared" ref="R69:R103" si="3">(D69-L69)/D69</f>
+        <f t="shared" ref="R69:R103" si="9">(D69-L69)/D69</f>
         <v>0.25</v>
       </c>
     </row>
@@ -9551,19 +9554,19 @@
         <v>8</v>
       </c>
       <c r="N70" s="2">
-        <f>(C70-G70)/C70</f>
+        <f t="shared" si="6"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O70" s="2">
-        <f>(D70-H70)/D70</f>
+        <f t="shared" si="7"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q70" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R70" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -9596,19 +9599,19 @@
         <v>9</v>
       </c>
       <c r="N71" s="2">
-        <f>(C71-G71)/C71</f>
+        <f t="shared" si="6"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O71" s="2">
-        <f>(D71-H71)/D71</f>
+        <f t="shared" si="7"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q71" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R71" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -9641,19 +9644,19 @@
         <v>9</v>
       </c>
       <c r="N72" s="2">
-        <f>(C72-G72)/C72</f>
+        <f t="shared" si="6"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O72" s="2">
-        <f>(D72-H72)/D72</f>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q72" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R72" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
     </row>
@@ -9686,19 +9689,19 @@
         <v>9</v>
       </c>
       <c r="N73" s="2">
-        <f>(C73-G73)/C73</f>
+        <f t="shared" si="6"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O73" s="2">
-        <f>(D73-H73)/D73</f>
+        <f t="shared" si="7"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q73" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R73" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -9731,19 +9734,19 @@
         <v>8</v>
       </c>
       <c r="N74" s="2">
-        <f>(C74-G74)/C74</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O74" s="2">
-        <f>(D74-H74)/D74</f>
+        <f t="shared" si="7"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q74" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="R74" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -9776,19 +9779,19 @@
         <v>9</v>
       </c>
       <c r="N75" s="2">
-        <f>(C75-G75)/C75</f>
+        <f t="shared" si="6"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O75" s="2">
-        <f>(D75-H75)/D75</f>
+        <f t="shared" si="7"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q75" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="R75" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -9821,19 +9824,19 @@
         <v>7</v>
       </c>
       <c r="N76" s="2">
-        <f>(C76-G76)/C76</f>
+        <f t="shared" si="6"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O76" s="2">
-        <f>(D76-H76)/D76</f>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q76" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R76" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.46153846153846156</v>
       </c>
     </row>
@@ -9866,19 +9869,19 @@
         <v>9</v>
       </c>
       <c r="N77" s="2">
-        <f>(C77-G77)/C77</f>
+        <f t="shared" si="6"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O77" s="2">
-        <f>(D77-H77)/D77</f>
+        <f t="shared" si="7"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q77" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R77" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -9911,19 +9914,19 @@
         <v>7</v>
       </c>
       <c r="N78" s="2">
-        <f>(C78-G78)/C78</f>
+        <f t="shared" si="6"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O78" s="2">
-        <f>(D78-H78)/D78</f>
+        <f t="shared" si="7"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q78" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R78" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.36363636363636365</v>
       </c>
     </row>
@@ -9956,19 +9959,19 @@
         <v>9</v>
       </c>
       <c r="N79" s="2">
-        <f>(C79-G79)/C79</f>
+        <f t="shared" si="6"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O79" s="2">
-        <f>(D79-H79)/D79</f>
+        <f t="shared" si="7"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q79" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R79" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -10001,19 +10004,19 @@
         <v>8</v>
       </c>
       <c r="N80" s="2">
-        <f>(C80-G80)/C80</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O80" s="2">
-        <f>(D80-H80)/D80</f>
+        <f t="shared" si="7"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Q80" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="R80" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -10046,19 +10049,19 @@
         <v>9</v>
       </c>
       <c r="N81" s="2">
-        <f>(C81-G81)/C81</f>
+        <f t="shared" si="6"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O81" s="2">
-        <f>(D81-H81)/D81</f>
+        <f t="shared" si="7"/>
         <v>0.7</v>
       </c>
       <c r="Q81" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.2608695652173913</v>
       </c>
       <c r="R81" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.1</v>
       </c>
     </row>
@@ -10091,19 +10094,19 @@
         <v>9</v>
       </c>
       <c r="N82" s="2">
-        <f>(C82-G82)/C82</f>
+        <f t="shared" si="6"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O82" s="2">
-        <f>(D82-H82)/D82</f>
+        <f t="shared" si="7"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q82" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R82" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -10136,19 +10139,19 @@
         <v>8</v>
       </c>
       <c r="N83" s="2">
-        <f>(C83-G83)/C83</f>
+        <f t="shared" si="6"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O83" s="2">
-        <f>(D83-H83)/D83</f>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q83" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R83" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -10181,19 +10184,19 @@
         <v>7</v>
       </c>
       <c r="N84" s="2">
-        <f>(C84-G84)/C84</f>
+        <f t="shared" si="6"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O84" s="2">
-        <f>(D84-H84)/D84</f>
+        <f t="shared" si="7"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q84" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R84" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.36363636363636365</v>
       </c>
     </row>
@@ -10226,19 +10229,19 @@
         <v>7</v>
       </c>
       <c r="N85" s="2">
-        <f>(C85-G85)/C85</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O85" s="2">
-        <f>(D85-H85)/D85</f>
+        <f t="shared" si="7"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q85" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R85" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.36363636363636365</v>
       </c>
     </row>
@@ -10271,19 +10274,19 @@
         <v>8</v>
       </c>
       <c r="N86" s="2">
-        <f>(C86-G86)/C86</f>
+        <f t="shared" si="6"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O86" s="2">
-        <f>(D86-H86)/D86</f>
+        <f t="shared" si="7"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q86" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R86" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -10316,19 +10319,19 @@
         <v>8</v>
       </c>
       <c r="N87" s="2">
-        <f>(C87-G87)/C87</f>
+        <f t="shared" si="6"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O87" s="2">
-        <f>(D87-H87)/D87</f>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q87" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.19047619047619047</v>
       </c>
       <c r="R87" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -10361,19 +10364,19 @@
         <v>8</v>
       </c>
       <c r="N88" s="2">
-        <f>(C88-G88)/C88</f>
+        <f t="shared" si="6"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O88" s="2">
-        <f>(D88-H88)/D88</f>
+        <f t="shared" si="7"/>
         <v>0.7</v>
       </c>
       <c r="Q88" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R88" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
     </row>
@@ -10406,19 +10409,19 @@
         <v>8</v>
       </c>
       <c r="N89" s="2">
-        <f>(C89-G89)/C89</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O89" s="2">
-        <f>(D89-H89)/D89</f>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q89" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R89" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -10451,19 +10454,19 @@
         <v>9</v>
       </c>
       <c r="N90" s="2">
-        <f>(C90-G90)/C90</f>
+        <f t="shared" si="6"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="O90" s="2">
-        <f>(D90-H90)/D90</f>
+        <f t="shared" si="7"/>
         <v>0.72727272727272729</v>
       </c>
       <c r="Q90" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R90" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -10496,19 +10499,19 @@
         <v>9</v>
       </c>
       <c r="N91" s="2">
-        <f>(C91-G91)/C91</f>
+        <f t="shared" si="6"/>
         <v>0.34782608695652173</v>
       </c>
       <c r="O91" s="2">
-        <f>(D91-H91)/D91</f>
+        <f t="shared" si="7"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="Q91" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.17391304347826086</v>
       </c>
       <c r="R91" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.18181818181818182</v>
       </c>
     </row>
@@ -10541,19 +10544,19 @@
         <v>9</v>
       </c>
       <c r="N92" s="2">
-        <f>(C92-G92)/C92</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O92" s="2">
-        <f>(D92-H92)/D92</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="Q92" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>9.5238095238095233E-2</v>
       </c>
       <c r="R92" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
     </row>
@@ -10586,19 +10589,19 @@
         <v>8</v>
       </c>
       <c r="N93" s="2">
-        <f>(C93-G93)/C93</f>
+        <f t="shared" si="6"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O93" s="2">
-        <f>(D93-H93)/D93</f>
+        <f t="shared" si="7"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="Q93" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="R93" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -10631,19 +10634,19 @@
         <v>7</v>
       </c>
       <c r="N94" s="2">
-        <f>(C94-G94)/C94</f>
+        <f t="shared" si="6"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O94" s="2">
-        <f>(D94-H94)/D94</f>
+        <f t="shared" si="7"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Q94" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.21739130434782608</v>
       </c>
       <c r="R94" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
     </row>
@@ -10676,19 +10679,19 @@
         <v>7</v>
       </c>
       <c r="N95" s="2">
-        <f>(C95-G95)/C95</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O95" s="2">
-        <f>(D95-H95)/D95</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="Q95" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R95" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -10721,19 +10724,19 @@
         <v>8</v>
       </c>
       <c r="N96" s="2">
-        <f>(C96-G96)/C96</f>
+        <f t="shared" si="6"/>
         <v>0.39130434782608697</v>
       </c>
       <c r="O96" s="2">
-        <f>(D96-H96)/D96</f>
+        <f t="shared" si="7"/>
         <v>0.69230769230769229</v>
       </c>
       <c r="Q96" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.2608695652173913</v>
       </c>
       <c r="R96" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.38461538461538464</v>
       </c>
     </row>
@@ -10766,19 +10769,19 @@
         <v>9</v>
       </c>
       <c r="N97" s="2">
-        <f>(C97-G97)/C97</f>
+        <f t="shared" si="6"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="O97" s="2">
-        <f>(D97-H97)/D97</f>
+        <f t="shared" si="7"/>
         <v>0.7857142857142857</v>
       </c>
       <c r="Q97" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R97" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.35714285714285715</v>
       </c>
     </row>
@@ -10811,19 +10814,19 @@
         <v>8</v>
       </c>
       <c r="N98" s="2">
-        <f>(C98-G98)/C98</f>
+        <f t="shared" si="6"/>
         <v>0.40909090909090912</v>
       </c>
       <c r="O98" s="2">
-        <f>(D98-H98)/D98</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="Q98" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="R98" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
     </row>
@@ -10856,19 +10859,19 @@
         <v>8</v>
       </c>
       <c r="N99" s="2">
-        <f>(C99-G99)/C99</f>
+        <f t="shared" si="6"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="O99" s="2">
-        <f>(D99-H99)/D99</f>
+        <f t="shared" si="7"/>
         <v>0.7</v>
       </c>
       <c r="Q99" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="R99" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.2</v>
       </c>
     </row>
@@ -10901,19 +10904,19 @@
         <v>8</v>
       </c>
       <c r="N100" s="2">
-        <f>(C100-G100)/C100</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O100" s="2">
-        <f>(D100-H100)/D100</f>
+        <f t="shared" si="7"/>
         <v>0.58333333333333337</v>
       </c>
       <c r="Q100" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R100" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -10946,19 +10949,19 @@
         <v>9</v>
       </c>
       <c r="N101" s="2">
-        <f>(C101-G101)/C101</f>
+        <f t="shared" si="6"/>
         <v>0.43478260869565216</v>
       </c>
       <c r="O101" s="2">
-        <f>(D101-H101)/D101</f>
+        <f t="shared" si="7"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="Q101" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.30434782608695654</v>
       </c>
       <c r="R101" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.30769230769230771</v>
       </c>
     </row>
@@ -10991,19 +10994,19 @@
         <v>9</v>
       </c>
       <c r="N102" s="2">
-        <f>(C102-G102)/C102</f>
+        <f t="shared" si="6"/>
         <v>0.2857142857142857</v>
       </c>
       <c r="O102" s="2">
-        <f>(D102-H102)/D102</f>
+        <f t="shared" si="7"/>
         <v>0.75</v>
       </c>
       <c r="Q102" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="R102" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.25</v>
       </c>
     </row>
@@ -11036,19 +11039,19 @@
         <v>7</v>
       </c>
       <c r="N103" s="2">
-        <f>(C103-G103)/C103</f>
+        <f t="shared" si="6"/>
         <v>0.38095238095238093</v>
       </c>
       <c r="O103" s="2">
-        <f>(D103-H103)/D103</f>
+        <f t="shared" si="7"/>
         <v>0.6</v>
       </c>
       <c r="Q103" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0.23809523809523808</v>
       </c>
       <c r="R103" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.3</v>
       </c>
     </row>

</xml_diff>